<commit_message>
updated UI for section 6a
</commit_message>
<xml_diff>
--- a/tests/calculator-cases.xlsx
+++ b/tests/calculator-cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="1120" windowWidth="28220" windowHeight="16260" tabRatio="972"/>
+    <workbookView xWindow="36120" yWindow="1120" windowWidth="28220" windowHeight="16260" tabRatio="972" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Section III (Method A.1)" sheetId="6" r:id="rId1"/>
@@ -7197,51 +7197,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7261,6 +7216,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7298,6 +7268,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1303">
@@ -9174,7 +9174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9188,7 +9188,7 @@
   </sheetPr>
   <dimension ref="A1:CH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="X13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -13247,7 +13247,6 @@
     <mergeCell ref="A2:BJ2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -17399,7 +17398,6 @@
     <mergeCell ref="A3:Y3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -27181,7 +27179,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -42384,7 +42381,7 @@
   </sheetPr>
   <dimension ref="A2:AY41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -42446,48 +42443,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:45" ht="30">
-      <c r="A2" s="248" t="s">
+      <c r="A2" s="233" t="s">
         <v>580</v>
       </c>
-      <c r="B2" s="248"/>
-      <c r="C2" s="248"/>
-      <c r="D2" s="248"/>
-      <c r="E2" s="248"/>
-      <c r="F2" s="248"/>
-      <c r="G2" s="248"/>
-      <c r="H2" s="248"/>
-      <c r="I2" s="248"/>
-      <c r="J2" s="248"/>
-      <c r="K2" s="248"/>
-      <c r="L2" s="248"/>
-      <c r="M2" s="248"/>
-      <c r="N2" s="248"/>
-      <c r="O2" s="248"/>
+      <c r="B2" s="233"/>
+      <c r="C2" s="233"/>
+      <c r="D2" s="233"/>
+      <c r="E2" s="233"/>
+      <c r="F2" s="233"/>
+      <c r="G2" s="233"/>
+      <c r="H2" s="233"/>
+      <c r="I2" s="233"/>
+      <c r="J2" s="233"/>
+      <c r="K2" s="233"/>
+      <c r="L2" s="233"/>
+      <c r="M2" s="233"/>
+      <c r="N2" s="233"/>
+      <c r="O2" s="233"/>
     </row>
     <row r="3" spans="1:45" ht="15" thickBot="1"/>
     <row r="4" spans="1:45" s="16" customFormat="1" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A4" s="253" t="s">
+      <c r="A4" s="243" t="s">
         <v>579</v>
       </c>
-      <c r="B4" s="254"/>
-      <c r="C4" s="254"/>
-      <c r="D4" s="254"/>
-      <c r="E4" s="254"/>
-      <c r="F4" s="254"/>
-      <c r="G4" s="254"/>
-      <c r="H4" s="254"/>
-      <c r="I4" s="254"/>
-      <c r="J4" s="254"/>
-      <c r="K4" s="254"/>
-      <c r="L4" s="254"/>
-      <c r="M4" s="254"/>
-      <c r="N4" s="254"/>
-      <c r="O4" s="254"/>
-      <c r="P4" s="254"/>
-      <c r="Q4" s="254"/>
-      <c r="R4" s="254"/>
-      <c r="S4" s="254"/>
-      <c r="T4" s="255"/>
+      <c r="B4" s="244"/>
+      <c r="C4" s="244"/>
+      <c r="D4" s="244"/>
+      <c r="E4" s="244"/>
+      <c r="F4" s="244"/>
+      <c r="G4" s="244"/>
+      <c r="H4" s="244"/>
+      <c r="I4" s="244"/>
+      <c r="J4" s="244"/>
+      <c r="K4" s="244"/>
+      <c r="L4" s="244"/>
+      <c r="M4" s="244"/>
+      <c r="N4" s="244"/>
+      <c r="O4" s="244"/>
+      <c r="P4" s="244"/>
+      <c r="Q4" s="244"/>
+      <c r="R4" s="244"/>
+      <c r="S4" s="244"/>
+      <c r="T4" s="245"/>
     </row>
     <row r="5" spans="1:45" s="16" customFormat="1" ht="56">
       <c r="A5" s="70"/>
@@ -42688,18 +42685,18 @@
       <c r="J8" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="249" t="s">
+      <c r="K8" s="234" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="250"/>
-      <c r="M8" s="250"/>
-      <c r="N8" s="250"/>
-      <c r="O8" s="250"/>
-      <c r="P8" s="250"/>
-      <c r="Q8" s="250"/>
-      <c r="R8" s="250"/>
-      <c r="S8" s="250"/>
-      <c r="T8" s="251"/>
+      <c r="L8" s="235"/>
+      <c r="M8" s="235"/>
+      <c r="N8" s="235"/>
+      <c r="O8" s="235"/>
+      <c r="P8" s="235"/>
+      <c r="Q8" s="235"/>
+      <c r="R8" s="235"/>
+      <c r="S8" s="235"/>
+      <c r="T8" s="236"/>
     </row>
     <row r="9" spans="1:45" s="16" customFormat="1" ht="81" customHeight="1" thickBot="1">
       <c r="A9" s="50"/>
@@ -42758,23 +42755,23 @@
       <c r="AF10" s="25"/>
     </row>
     <row r="11" spans="1:45" ht="29" thickBot="1">
-      <c r="A11" s="230" t="s">
+      <c r="A11" s="257" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="231"/>
-      <c r="C11" s="231"/>
-      <c r="D11" s="231"/>
-      <c r="E11" s="231"/>
-      <c r="F11" s="231"/>
-      <c r="G11" s="231"/>
-      <c r="H11" s="231"/>
-      <c r="I11" s="231"/>
-      <c r="J11" s="231"/>
-      <c r="K11" s="231"/>
-      <c r="L11" s="231"/>
-      <c r="M11" s="231"/>
-      <c r="N11" s="231"/>
-      <c r="O11" s="232"/>
+      <c r="B11" s="258"/>
+      <c r="C11" s="258"/>
+      <c r="D11" s="258"/>
+      <c r="E11" s="258"/>
+      <c r="F11" s="258"/>
+      <c r="G11" s="258"/>
+      <c r="H11" s="258"/>
+      <c r="I11" s="258"/>
+      <c r="J11" s="258"/>
+      <c r="K11" s="258"/>
+      <c r="L11" s="258"/>
+      <c r="M11" s="258"/>
+      <c r="N11" s="258"/>
+      <c r="O11" s="259"/>
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
@@ -42826,23 +42823,23 @@
       <c r="AS12" s="26"/>
     </row>
     <row r="13" spans="1:45" s="22" customFormat="1" ht="31" thickBot="1">
-      <c r="A13" s="233" t="s">
+      <c r="A13" s="254" t="s">
         <v>322</v>
       </c>
-      <c r="B13" s="234"/>
-      <c r="C13" s="234"/>
-      <c r="D13" s="234"/>
-      <c r="E13" s="234"/>
-      <c r="F13" s="234"/>
-      <c r="G13" s="234"/>
-      <c r="H13" s="234"/>
-      <c r="I13" s="234"/>
-      <c r="J13" s="234"/>
-      <c r="K13" s="234"/>
-      <c r="L13" s="234"/>
-      <c r="M13" s="234"/>
-      <c r="N13" s="234"/>
-      <c r="O13" s="235"/>
+      <c r="B13" s="255"/>
+      <c r="C13" s="255"/>
+      <c r="D13" s="255"/>
+      <c r="E13" s="255"/>
+      <c r="F13" s="255"/>
+      <c r="G13" s="255"/>
+      <c r="H13" s="255"/>
+      <c r="I13" s="255"/>
+      <c r="J13" s="255"/>
+      <c r="K13" s="255"/>
+      <c r="L13" s="255"/>
+      <c r="M13" s="255"/>
+      <c r="N13" s="255"/>
+      <c r="O13" s="256"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
       <c r="R13" s="26"/>
@@ -42871,31 +42868,31 @@
       <c r="AO13" s="26"/>
     </row>
     <row r="14" spans="1:45" s="22" customFormat="1" ht="24" thickBot="1">
-      <c r="A14" s="244" t="s">
+      <c r="A14" s="239" t="s">
         <v>331</v>
       </c>
-      <c r="B14" s="242"/>
-      <c r="C14" s="242"/>
-      <c r="D14" s="243"/>
-      <c r="E14" s="239" t="s">
+      <c r="B14" s="240"/>
+      <c r="C14" s="240"/>
+      <c r="D14" s="241"/>
+      <c r="E14" s="237" t="s">
         <v>334</v>
       </c>
-      <c r="F14" s="241" t="s">
+      <c r="F14" s="263" t="s">
         <v>332</v>
       </c>
-      <c r="G14" s="242"/>
-      <c r="H14" s="242"/>
-      <c r="I14" s="242"/>
-      <c r="J14" s="239" t="s">
+      <c r="G14" s="240"/>
+      <c r="H14" s="240"/>
+      <c r="I14" s="240"/>
+      <c r="J14" s="237" t="s">
         <v>334</v>
       </c>
-      <c r="K14" s="256" t="s">
+      <c r="K14" s="246" t="s">
         <v>333</v>
       </c>
-      <c r="L14" s="256"/>
-      <c r="M14" s="256"/>
-      <c r="N14" s="256"/>
-      <c r="O14" s="257"/>
+      <c r="L14" s="246"/>
+      <c r="M14" s="246"/>
+      <c r="N14" s="246"/>
+      <c r="O14" s="247"/>
       <c r="P14" s="27"/>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -42934,7 +42931,7 @@
         <v>397</v>
       </c>
       <c r="D15" s="85"/>
-      <c r="E15" s="239"/>
+      <c r="E15" s="237"/>
       <c r="F15" s="79" t="s">
         <v>396</v>
       </c>
@@ -42945,7 +42942,7 @@
         <v>397</v>
       </c>
       <c r="I15" s="84"/>
-      <c r="J15" s="239"/>
+      <c r="J15" s="237"/>
       <c r="K15" s="79" t="s">
         <v>578</v>
       </c>
@@ -42999,7 +42996,7 @@
       <c r="D16" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="239"/>
+      <c r="E16" s="237"/>
       <c r="F16" s="34" t="s">
         <v>16</v>
       </c>
@@ -43012,7 +43009,7 @@
       <c r="I16" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="239"/>
+      <c r="J16" s="237"/>
       <c r="K16" s="34" t="s">
         <v>18</v>
       </c>
@@ -43065,7 +43062,7 @@
       <c r="D17" s="38">
         <v>4</v>
       </c>
-      <c r="E17" s="239"/>
+      <c r="E17" s="237"/>
       <c r="F17" s="17">
         <v>35</v>
       </c>
@@ -43078,7 +43075,7 @@
       <c r="I17" s="38">
         <v>4</v>
       </c>
-      <c r="J17" s="239"/>
+      <c r="J17" s="237"/>
       <c r="K17" s="17">
         <v>2.5</v>
       </c>
@@ -43119,30 +43116,30 @@
       <c r="AL17" s="26"/>
     </row>
     <row r="18" spans="1:51" s="22" customFormat="1" ht="29" thickBot="1">
-      <c r="A18" s="258" t="s">
+      <c r="A18" s="248" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="252"/>
-      <c r="C18" s="252"/>
+      <c r="B18" s="242"/>
+      <c r="C18" s="242"/>
       <c r="D18" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="240"/>
-      <c r="F18" s="252" t="s">
+      <c r="E18" s="238"/>
+      <c r="F18" s="242" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="252"/>
-      <c r="H18" s="252"/>
+      <c r="G18" s="242"/>
+      <c r="H18" s="242"/>
       <c r="I18" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="240"/>
-      <c r="K18" s="259" t="s">
+      <c r="J18" s="238"/>
+      <c r="K18" s="249" t="s">
         <v>38</v>
       </c>
-      <c r="L18" s="259"/>
-      <c r="M18" s="259"/>
-      <c r="N18" s="259"/>
+      <c r="L18" s="249"/>
+      <c r="M18" s="249"/>
+      <c r="N18" s="249"/>
       <c r="O18" s="46" t="s">
         <v>36</v>
       </c>
@@ -43171,24 +43168,24 @@
       <c r="AL18" s="26"/>
     </row>
     <row r="19" spans="1:51" s="22" customFormat="1">
-      <c r="A19" s="260" t="s">
+      <c r="A19" s="250" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="261"/>
-      <c r="C19" s="261"/>
-      <c r="D19" s="261"/>
-      <c r="E19" s="261"/>
-      <c r="F19" s="261"/>
-      <c r="G19" s="261"/>
-      <c r="H19" s="261"/>
-      <c r="I19" s="261"/>
-      <c r="J19" s="261"/>
-      <c r="K19" s="261"/>
-      <c r="L19" s="261"/>
-      <c r="M19" s="261"/>
-      <c r="N19" s="261"/>
-      <c r="O19" s="261"/>
-      <c r="P19" s="262"/>
+      <c r="B19" s="251"/>
+      <c r="C19" s="251"/>
+      <c r="D19" s="251"/>
+      <c r="E19" s="251"/>
+      <c r="F19" s="251"/>
+      <c r="G19" s="251"/>
+      <c r="H19" s="251"/>
+      <c r="I19" s="251"/>
+      <c r="J19" s="251"/>
+      <c r="K19" s="251"/>
+      <c r="L19" s="251"/>
+      <c r="M19" s="251"/>
+      <c r="N19" s="251"/>
+      <c r="O19" s="251"/>
+      <c r="P19" s="252"/>
       <c r="Q19" s="26"/>
       <c r="R19" s="26"/>
       <c r="S19" s="26"/>
@@ -43216,78 +43213,78 @@
       <c r="AO19" s="26"/>
     </row>
     <row r="20" spans="1:51" ht="15" thickBot="1">
-      <c r="A20" s="260"/>
-      <c r="B20" s="261"/>
-      <c r="C20" s="261"/>
-      <c r="D20" s="261"/>
-      <c r="E20" s="261"/>
-      <c r="F20" s="261"/>
-      <c r="G20" s="261"/>
-      <c r="H20" s="261"/>
-      <c r="I20" s="261"/>
-      <c r="J20" s="261"/>
-      <c r="K20" s="261"/>
-      <c r="L20" s="261"/>
-      <c r="M20" s="261"/>
-      <c r="N20" s="261"/>
-      <c r="O20" s="261"/>
-      <c r="P20" s="263"/>
+      <c r="A20" s="250"/>
+      <c r="B20" s="251"/>
+      <c r="C20" s="251"/>
+      <c r="D20" s="251"/>
+      <c r="E20" s="251"/>
+      <c r="F20" s="251"/>
+      <c r="G20" s="251"/>
+      <c r="H20" s="251"/>
+      <c r="I20" s="251"/>
+      <c r="J20" s="251"/>
+      <c r="K20" s="251"/>
+      <c r="L20" s="251"/>
+      <c r="M20" s="251"/>
+      <c r="N20" s="251"/>
+      <c r="O20" s="251"/>
+      <c r="P20" s="253"/>
       <c r="AP20"/>
       <c r="AQ20"/>
       <c r="AR20"/>
       <c r="AS20"/>
     </row>
     <row r="21" spans="1:51" ht="31" thickBot="1">
-      <c r="A21" s="233" t="s">
+      <c r="A21" s="254" t="s">
         <v>323</v>
       </c>
-      <c r="B21" s="234"/>
-      <c r="C21" s="234"/>
-      <c r="D21" s="234"/>
-      <c r="E21" s="234"/>
-      <c r="F21" s="234"/>
-      <c r="G21" s="234"/>
-      <c r="H21" s="234"/>
-      <c r="I21" s="234"/>
-      <c r="J21" s="234"/>
-      <c r="K21" s="234"/>
-      <c r="L21" s="234"/>
-      <c r="M21" s="234"/>
-      <c r="N21" s="234"/>
-      <c r="O21" s="234"/>
-      <c r="P21" s="235"/>
+      <c r="B21" s="255"/>
+      <c r="C21" s="255"/>
+      <c r="D21" s="255"/>
+      <c r="E21" s="255"/>
+      <c r="F21" s="255"/>
+      <c r="G21" s="255"/>
+      <c r="H21" s="255"/>
+      <c r="I21" s="255"/>
+      <c r="J21" s="255"/>
+      <c r="K21" s="255"/>
+      <c r="L21" s="255"/>
+      <c r="M21" s="255"/>
+      <c r="N21" s="255"/>
+      <c r="O21" s="255"/>
+      <c r="P21" s="256"/>
       <c r="AP21"/>
       <c r="AQ21"/>
       <c r="AR21"/>
       <c r="AS21"/>
     </row>
     <row r="22" spans="1:51" ht="24" thickBot="1">
-      <c r="A22" s="244" t="s">
+      <c r="A22" s="239" t="s">
         <v>331</v>
       </c>
-      <c r="B22" s="242"/>
-      <c r="C22" s="243"/>
-      <c r="D22" s="239" t="s">
+      <c r="B22" s="240"/>
+      <c r="C22" s="241"/>
+      <c r="D22" s="237" t="s">
         <v>334</v>
       </c>
-      <c r="E22" s="241" t="s">
+      <c r="E22" s="263" t="s">
         <v>332</v>
       </c>
-      <c r="F22" s="242"/>
-      <c r="G22" s="242"/>
-      <c r="H22" s="242"/>
-      <c r="I22" s="243"/>
-      <c r="J22" s="239" t="s">
+      <c r="F22" s="240"/>
+      <c r="G22" s="240"/>
+      <c r="H22" s="240"/>
+      <c r="I22" s="241"/>
+      <c r="J22" s="237" t="s">
         <v>334</v>
       </c>
-      <c r="K22" s="236" t="s">
+      <c r="K22" s="260" t="s">
         <v>333</v>
       </c>
-      <c r="L22" s="237"/>
-      <c r="M22" s="237"/>
-      <c r="N22" s="237"/>
-      <c r="O22" s="237"/>
-      <c r="P22" s="238"/>
+      <c r="L22" s="261"/>
+      <c r="M22" s="261"/>
+      <c r="N22" s="261"/>
+      <c r="O22" s="261"/>
+      <c r="P22" s="262"/>
       <c r="AM22"/>
       <c r="AN22"/>
       <c r="AO22"/>
@@ -43306,7 +43303,7 @@
       <c r="C23" s="79" t="s">
         <v>397</v>
       </c>
-      <c r="D23" s="239"/>
+      <c r="D23" s="237"/>
       <c r="E23" s="79" t="s">
         <v>396</v>
       </c>
@@ -43318,7 +43315,7 @@
       </c>
       <c r="H23" s="84"/>
       <c r="I23" s="85"/>
-      <c r="J23" s="239"/>
+      <c r="J23" s="237"/>
       <c r="K23" s="79" t="s">
         <v>578</v>
       </c>
@@ -43351,7 +43348,7 @@
       <c r="C24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="239"/>
+      <c r="D24" s="237"/>
       <c r="E24" s="34" t="s">
         <v>16</v>
       </c>
@@ -43367,7 +43364,7 @@
       <c r="I24" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J24" s="239"/>
+      <c r="J24" s="237"/>
       <c r="K24" s="34" t="s">
         <v>18</v>
       </c>
@@ -43403,7 +43400,7 @@
       <c r="C25" s="17">
         <v>45</v>
       </c>
-      <c r="D25" s="239"/>
+      <c r="D25" s="237"/>
       <c r="E25" s="17">
         <v>35</v>
       </c>
@@ -43419,7 +43416,7 @@
       <c r="I25" s="17">
         <v>95</v>
       </c>
-      <c r="J25" s="239"/>
+      <c r="J25" s="237"/>
       <c r="K25" s="17">
         <v>2.5</v>
       </c>
@@ -43446,30 +43443,30 @@
       <c r="AS25"/>
     </row>
     <row r="26" spans="1:51" ht="50.25" customHeight="1" thickBot="1">
-      <c r="A26" s="258" t="s">
+      <c r="A26" s="248" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="252"/>
-      <c r="C26" s="252"/>
-      <c r="D26" s="240"/>
-      <c r="E26" s="252" t="s">
+      <c r="B26" s="242"/>
+      <c r="C26" s="242"/>
+      <c r="D26" s="238"/>
+      <c r="E26" s="242" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="252"/>
-      <c r="G26" s="252"/>
+      <c r="F26" s="242"/>
+      <c r="G26" s="242"/>
       <c r="H26" s="45" t="s">
         <v>36</v>
       </c>
       <c r="I26" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="J26" s="240"/>
-      <c r="K26" s="259" t="s">
+      <c r="J26" s="238"/>
+      <c r="K26" s="249" t="s">
         <v>38</v>
       </c>
-      <c r="L26" s="259"/>
-      <c r="M26" s="259"/>
-      <c r="N26" s="259"/>
+      <c r="L26" s="249"/>
+      <c r="M26" s="249"/>
+      <c r="N26" s="249"/>
       <c r="O26" s="45" t="s">
         <v>36</v>
       </c>
@@ -43490,53 +43487,53 @@
     </row>
     <row r="29" spans="1:51" ht="15" thickBot="1"/>
     <row r="30" spans="1:51" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A30" s="245" t="s">
+      <c r="A30" s="230" t="s">
         <v>576</v>
       </c>
-      <c r="B30" s="246"/>
-      <c r="C30" s="246"/>
-      <c r="D30" s="246"/>
-      <c r="E30" s="246"/>
-      <c r="F30" s="246"/>
-      <c r="G30" s="246"/>
-      <c r="H30" s="246"/>
-      <c r="I30" s="246"/>
-      <c r="J30" s="246"/>
-      <c r="K30" s="246"/>
-      <c r="L30" s="246"/>
-      <c r="M30" s="246"/>
-      <c r="N30" s="246"/>
-      <c r="O30" s="246"/>
-      <c r="P30" s="246"/>
-      <c r="Q30" s="246"/>
-      <c r="R30" s="246"/>
-      <c r="S30" s="246"/>
-      <c r="T30" s="246"/>
-      <c r="U30" s="246"/>
-      <c r="V30" s="246"/>
-      <c r="W30" s="246"/>
-      <c r="X30" s="246"/>
-      <c r="Y30" s="246"/>
-      <c r="Z30" s="246"/>
-      <c r="AA30" s="246"/>
-      <c r="AB30" s="246"/>
-      <c r="AC30" s="246"/>
-      <c r="AD30" s="246"/>
-      <c r="AE30" s="246"/>
-      <c r="AF30" s="246"/>
-      <c r="AG30" s="246"/>
-      <c r="AH30" s="246"/>
-      <c r="AI30" s="246"/>
-      <c r="AJ30" s="246"/>
-      <c r="AK30" s="246"/>
-      <c r="AL30" s="246"/>
-      <c r="AM30" s="246"/>
-      <c r="AN30" s="246"/>
-      <c r="AO30" s="246"/>
-      <c r="AP30" s="246"/>
-      <c r="AQ30" s="246"/>
-      <c r="AR30" s="246"/>
-      <c r="AS30" s="247"/>
+      <c r="B30" s="231"/>
+      <c r="C30" s="231"/>
+      <c r="D30" s="231"/>
+      <c r="E30" s="231"/>
+      <c r="F30" s="231"/>
+      <c r="G30" s="231"/>
+      <c r="H30" s="231"/>
+      <c r="I30" s="231"/>
+      <c r="J30" s="231"/>
+      <c r="K30" s="231"/>
+      <c r="L30" s="231"/>
+      <c r="M30" s="231"/>
+      <c r="N30" s="231"/>
+      <c r="O30" s="231"/>
+      <c r="P30" s="231"/>
+      <c r="Q30" s="231"/>
+      <c r="R30" s="231"/>
+      <c r="S30" s="231"/>
+      <c r="T30" s="231"/>
+      <c r="U30" s="231"/>
+      <c r="V30" s="231"/>
+      <c r="W30" s="231"/>
+      <c r="X30" s="231"/>
+      <c r="Y30" s="231"/>
+      <c r="Z30" s="231"/>
+      <c r="AA30" s="231"/>
+      <c r="AB30" s="231"/>
+      <c r="AC30" s="231"/>
+      <c r="AD30" s="231"/>
+      <c r="AE30" s="231"/>
+      <c r="AF30" s="231"/>
+      <c r="AG30" s="231"/>
+      <c r="AH30" s="231"/>
+      <c r="AI30" s="231"/>
+      <c r="AJ30" s="231"/>
+      <c r="AK30" s="231"/>
+      <c r="AL30" s="231"/>
+      <c r="AM30" s="231"/>
+      <c r="AN30" s="231"/>
+      <c r="AO30" s="231"/>
+      <c r="AP30" s="231"/>
+      <c r="AQ30" s="231"/>
+      <c r="AR30" s="231"/>
+      <c r="AS30" s="232"/>
     </row>
     <row r="31" spans="1:51" s="23" customFormat="1" ht="30.75" customHeight="1">
       <c r="A31" s="78" t="s">
@@ -44190,6 +44187,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="K22:P22"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="A30:AS30"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="K8:T8"/>
@@ -44206,14 +44211,6 @@
     <mergeCell ref="K18:N18"/>
     <mergeCell ref="A19:P20"/>
     <mergeCell ref="A21:P21"/>
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="K22:P22"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
hi er label complete
</commit_message>
<xml_diff>
--- a/tests/calculator-cases.xlsx
+++ b/tests/calculator-cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="1120" windowWidth="28220" windowHeight="16260" tabRatio="972" activeTab="7"/>
+    <workbookView xWindow="580" yWindow="0" windowWidth="28220" windowHeight="15940" tabRatio="972" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Section III (Method A.1)" sheetId="6" r:id="rId1"/>
@@ -5229,8 +5229,84 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1303">
+  <cellStyleXfs count="1379">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7197,6 +7273,51 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7216,21 +7337,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7269,38 +7375,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1303">
+  <cellStyles count="1379">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -7952,6 +8028,44 @@
     <cellStyle name="Followed Hyperlink" xfId="1298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1300" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1378" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -8603,6 +8717,44 @@
     <cellStyle name="Hyperlink" xfId="1297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1299" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1377" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
@@ -9174,7 +9326,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -22186,8 +22338,8 @@
   </sheetPr>
   <dimension ref="A1:CQ17"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D6:D17"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -27179,6 +27331,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -42381,7 +42534,7 @@
   </sheetPr>
   <dimension ref="A2:AY41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -42443,48 +42596,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:45" ht="30">
-      <c r="A2" s="233" t="s">
+      <c r="A2" s="248" t="s">
         <v>580</v>
       </c>
-      <c r="B2" s="233"/>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
-      <c r="I2" s="233"/>
-      <c r="J2" s="233"/>
-      <c r="K2" s="233"/>
-      <c r="L2" s="233"/>
-      <c r="M2" s="233"/>
-      <c r="N2" s="233"/>
-      <c r="O2" s="233"/>
+      <c r="B2" s="248"/>
+      <c r="C2" s="248"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="248"/>
+      <c r="F2" s="248"/>
+      <c r="G2" s="248"/>
+      <c r="H2" s="248"/>
+      <c r="I2" s="248"/>
+      <c r="J2" s="248"/>
+      <c r="K2" s="248"/>
+      <c r="L2" s="248"/>
+      <c r="M2" s="248"/>
+      <c r="N2" s="248"/>
+      <c r="O2" s="248"/>
     </row>
     <row r="3" spans="1:45" ht="15" thickBot="1"/>
     <row r="4" spans="1:45" s="16" customFormat="1" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A4" s="243" t="s">
+      <c r="A4" s="253" t="s">
         <v>579</v>
       </c>
-      <c r="B4" s="244"/>
-      <c r="C4" s="244"/>
-      <c r="D4" s="244"/>
-      <c r="E4" s="244"/>
-      <c r="F4" s="244"/>
-      <c r="G4" s="244"/>
-      <c r="H4" s="244"/>
-      <c r="I4" s="244"/>
-      <c r="J4" s="244"/>
-      <c r="K4" s="244"/>
-      <c r="L4" s="244"/>
-      <c r="M4" s="244"/>
-      <c r="N4" s="244"/>
-      <c r="O4" s="244"/>
-      <c r="P4" s="244"/>
-      <c r="Q4" s="244"/>
-      <c r="R4" s="244"/>
-      <c r="S4" s="244"/>
-      <c r="T4" s="245"/>
+      <c r="B4" s="254"/>
+      <c r="C4" s="254"/>
+      <c r="D4" s="254"/>
+      <c r="E4" s="254"/>
+      <c r="F4" s="254"/>
+      <c r="G4" s="254"/>
+      <c r="H4" s="254"/>
+      <c r="I4" s="254"/>
+      <c r="J4" s="254"/>
+      <c r="K4" s="254"/>
+      <c r="L4" s="254"/>
+      <c r="M4" s="254"/>
+      <c r="N4" s="254"/>
+      <c r="O4" s="254"/>
+      <c r="P4" s="254"/>
+      <c r="Q4" s="254"/>
+      <c r="R4" s="254"/>
+      <c r="S4" s="254"/>
+      <c r="T4" s="255"/>
     </row>
     <row r="5" spans="1:45" s="16" customFormat="1" ht="56">
       <c r="A5" s="70"/>
@@ -42685,18 +42838,18 @@
       <c r="J8" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="234" t="s">
+      <c r="K8" s="249" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="235"/>
-      <c r="M8" s="235"/>
-      <c r="N8" s="235"/>
-      <c r="O8" s="235"/>
-      <c r="P8" s="235"/>
-      <c r="Q8" s="235"/>
-      <c r="R8" s="235"/>
-      <c r="S8" s="235"/>
-      <c r="T8" s="236"/>
+      <c r="L8" s="250"/>
+      <c r="M8" s="250"/>
+      <c r="N8" s="250"/>
+      <c r="O8" s="250"/>
+      <c r="P8" s="250"/>
+      <c r="Q8" s="250"/>
+      <c r="R8" s="250"/>
+      <c r="S8" s="250"/>
+      <c r="T8" s="251"/>
     </row>
     <row r="9" spans="1:45" s="16" customFormat="1" ht="81" customHeight="1" thickBot="1">
       <c r="A9" s="50"/>
@@ -42755,23 +42908,23 @@
       <c r="AF10" s="25"/>
     </row>
     <row r="11" spans="1:45" ht="29" thickBot="1">
-      <c r="A11" s="257" t="s">
+      <c r="A11" s="230" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="258"/>
-      <c r="C11" s="258"/>
-      <c r="D11" s="258"/>
-      <c r="E11" s="258"/>
-      <c r="F11" s="258"/>
-      <c r="G11" s="258"/>
-      <c r="H11" s="258"/>
-      <c r="I11" s="258"/>
-      <c r="J11" s="258"/>
-      <c r="K11" s="258"/>
-      <c r="L11" s="258"/>
-      <c r="M11" s="258"/>
-      <c r="N11" s="258"/>
-      <c r="O11" s="259"/>
+      <c r="B11" s="231"/>
+      <c r="C11" s="231"/>
+      <c r="D11" s="231"/>
+      <c r="E11" s="231"/>
+      <c r="F11" s="231"/>
+      <c r="G11" s="231"/>
+      <c r="H11" s="231"/>
+      <c r="I11" s="231"/>
+      <c r="J11" s="231"/>
+      <c r="K11" s="231"/>
+      <c r="L11" s="231"/>
+      <c r="M11" s="231"/>
+      <c r="N11" s="231"/>
+      <c r="O11" s="232"/>
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
@@ -42823,23 +42976,23 @@
       <c r="AS12" s="26"/>
     </row>
     <row r="13" spans="1:45" s="22" customFormat="1" ht="31" thickBot="1">
-      <c r="A13" s="254" t="s">
+      <c r="A13" s="233" t="s">
         <v>322</v>
       </c>
-      <c r="B13" s="255"/>
-      <c r="C13" s="255"/>
-      <c r="D13" s="255"/>
-      <c r="E13" s="255"/>
-      <c r="F13" s="255"/>
-      <c r="G13" s="255"/>
-      <c r="H13" s="255"/>
-      <c r="I13" s="255"/>
-      <c r="J13" s="255"/>
-      <c r="K13" s="255"/>
-      <c r="L13" s="255"/>
-      <c r="M13" s="255"/>
-      <c r="N13" s="255"/>
-      <c r="O13" s="256"/>
+      <c r="B13" s="234"/>
+      <c r="C13" s="234"/>
+      <c r="D13" s="234"/>
+      <c r="E13" s="234"/>
+      <c r="F13" s="234"/>
+      <c r="G13" s="234"/>
+      <c r="H13" s="234"/>
+      <c r="I13" s="234"/>
+      <c r="J13" s="234"/>
+      <c r="K13" s="234"/>
+      <c r="L13" s="234"/>
+      <c r="M13" s="234"/>
+      <c r="N13" s="234"/>
+      <c r="O13" s="235"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
       <c r="R13" s="26"/>
@@ -42868,31 +43021,31 @@
       <c r="AO13" s="26"/>
     </row>
     <row r="14" spans="1:45" s="22" customFormat="1" ht="24" thickBot="1">
-      <c r="A14" s="239" t="s">
+      <c r="A14" s="244" t="s">
         <v>331</v>
       </c>
-      <c r="B14" s="240"/>
-      <c r="C14" s="240"/>
-      <c r="D14" s="241"/>
-      <c r="E14" s="237" t="s">
+      <c r="B14" s="242"/>
+      <c r="C14" s="242"/>
+      <c r="D14" s="243"/>
+      <c r="E14" s="239" t="s">
         <v>334</v>
       </c>
-      <c r="F14" s="263" t="s">
+      <c r="F14" s="241" t="s">
         <v>332</v>
       </c>
-      <c r="G14" s="240"/>
-      <c r="H14" s="240"/>
-      <c r="I14" s="240"/>
-      <c r="J14" s="237" t="s">
+      <c r="G14" s="242"/>
+      <c r="H14" s="242"/>
+      <c r="I14" s="242"/>
+      <c r="J14" s="239" t="s">
         <v>334</v>
       </c>
-      <c r="K14" s="246" t="s">
+      <c r="K14" s="256" t="s">
         <v>333</v>
       </c>
-      <c r="L14" s="246"/>
-      <c r="M14" s="246"/>
-      <c r="N14" s="246"/>
-      <c r="O14" s="247"/>
+      <c r="L14" s="256"/>
+      <c r="M14" s="256"/>
+      <c r="N14" s="256"/>
+      <c r="O14" s="257"/>
       <c r="P14" s="27"/>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -42931,7 +43084,7 @@
         <v>397</v>
       </c>
       <c r="D15" s="85"/>
-      <c r="E15" s="237"/>
+      <c r="E15" s="239"/>
       <c r="F15" s="79" t="s">
         <v>396</v>
       </c>
@@ -42942,7 +43095,7 @@
         <v>397</v>
       </c>
       <c r="I15" s="84"/>
-      <c r="J15" s="237"/>
+      <c r="J15" s="239"/>
       <c r="K15" s="79" t="s">
         <v>578</v>
       </c>
@@ -42996,7 +43149,7 @@
       <c r="D16" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="237"/>
+      <c r="E16" s="239"/>
       <c r="F16" s="34" t="s">
         <v>16</v>
       </c>
@@ -43009,7 +43162,7 @@
       <c r="I16" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="237"/>
+      <c r="J16" s="239"/>
       <c r="K16" s="34" t="s">
         <v>18</v>
       </c>
@@ -43062,7 +43215,7 @@
       <c r="D17" s="38">
         <v>4</v>
       </c>
-      <c r="E17" s="237"/>
+      <c r="E17" s="239"/>
       <c r="F17" s="17">
         <v>35</v>
       </c>
@@ -43075,7 +43228,7 @@
       <c r="I17" s="38">
         <v>4</v>
       </c>
-      <c r="J17" s="237"/>
+      <c r="J17" s="239"/>
       <c r="K17" s="17">
         <v>2.5</v>
       </c>
@@ -43116,30 +43269,30 @@
       <c r="AL17" s="26"/>
     </row>
     <row r="18" spans="1:51" s="22" customFormat="1" ht="29" thickBot="1">
-      <c r="A18" s="248" t="s">
+      <c r="A18" s="258" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="242"/>
-      <c r="C18" s="242"/>
+      <c r="B18" s="252"/>
+      <c r="C18" s="252"/>
       <c r="D18" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="238"/>
-      <c r="F18" s="242" t="s">
+      <c r="E18" s="240"/>
+      <c r="F18" s="252" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="242"/>
-      <c r="H18" s="242"/>
+      <c r="G18" s="252"/>
+      <c r="H18" s="252"/>
       <c r="I18" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="238"/>
-      <c r="K18" s="249" t="s">
+      <c r="J18" s="240"/>
+      <c r="K18" s="259" t="s">
         <v>38</v>
       </c>
-      <c r="L18" s="249"/>
-      <c r="M18" s="249"/>
-      <c r="N18" s="249"/>
+      <c r="L18" s="259"/>
+      <c r="M18" s="259"/>
+      <c r="N18" s="259"/>
       <c r="O18" s="46" t="s">
         <v>36</v>
       </c>
@@ -43168,24 +43321,24 @@
       <c r="AL18" s="26"/>
     </row>
     <row r="19" spans="1:51" s="22" customFormat="1">
-      <c r="A19" s="250" t="s">
+      <c r="A19" s="260" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="251"/>
-      <c r="C19" s="251"/>
-      <c r="D19" s="251"/>
-      <c r="E19" s="251"/>
-      <c r="F19" s="251"/>
-      <c r="G19" s="251"/>
-      <c r="H19" s="251"/>
-      <c r="I19" s="251"/>
-      <c r="J19" s="251"/>
-      <c r="K19" s="251"/>
-      <c r="L19" s="251"/>
-      <c r="M19" s="251"/>
-      <c r="N19" s="251"/>
-      <c r="O19" s="251"/>
-      <c r="P19" s="252"/>
+      <c r="B19" s="261"/>
+      <c r="C19" s="261"/>
+      <c r="D19" s="261"/>
+      <c r="E19" s="261"/>
+      <c r="F19" s="261"/>
+      <c r="G19" s="261"/>
+      <c r="H19" s="261"/>
+      <c r="I19" s="261"/>
+      <c r="J19" s="261"/>
+      <c r="K19" s="261"/>
+      <c r="L19" s="261"/>
+      <c r="M19" s="261"/>
+      <c r="N19" s="261"/>
+      <c r="O19" s="261"/>
+      <c r="P19" s="262"/>
       <c r="Q19" s="26"/>
       <c r="R19" s="26"/>
       <c r="S19" s="26"/>
@@ -43213,78 +43366,78 @@
       <c r="AO19" s="26"/>
     </row>
     <row r="20" spans="1:51" ht="15" thickBot="1">
-      <c r="A20" s="250"/>
-      <c r="B20" s="251"/>
-      <c r="C20" s="251"/>
-      <c r="D20" s="251"/>
-      <c r="E20" s="251"/>
-      <c r="F20" s="251"/>
-      <c r="G20" s="251"/>
-      <c r="H20" s="251"/>
-      <c r="I20" s="251"/>
-      <c r="J20" s="251"/>
-      <c r="K20" s="251"/>
-      <c r="L20" s="251"/>
-      <c r="M20" s="251"/>
-      <c r="N20" s="251"/>
-      <c r="O20" s="251"/>
-      <c r="P20" s="253"/>
+      <c r="A20" s="260"/>
+      <c r="B20" s="261"/>
+      <c r="C20" s="261"/>
+      <c r="D20" s="261"/>
+      <c r="E20" s="261"/>
+      <c r="F20" s="261"/>
+      <c r="G20" s="261"/>
+      <c r="H20" s="261"/>
+      <c r="I20" s="261"/>
+      <c r="J20" s="261"/>
+      <c r="K20" s="261"/>
+      <c r="L20" s="261"/>
+      <c r="M20" s="261"/>
+      <c r="N20" s="261"/>
+      <c r="O20" s="261"/>
+      <c r="P20" s="263"/>
       <c r="AP20"/>
       <c r="AQ20"/>
       <c r="AR20"/>
       <c r="AS20"/>
     </row>
     <row r="21" spans="1:51" ht="31" thickBot="1">
-      <c r="A21" s="254" t="s">
+      <c r="A21" s="233" t="s">
         <v>323</v>
       </c>
-      <c r="B21" s="255"/>
-      <c r="C21" s="255"/>
-      <c r="D21" s="255"/>
-      <c r="E21" s="255"/>
-      <c r="F21" s="255"/>
-      <c r="G21" s="255"/>
-      <c r="H21" s="255"/>
-      <c r="I21" s="255"/>
-      <c r="J21" s="255"/>
-      <c r="K21" s="255"/>
-      <c r="L21" s="255"/>
-      <c r="M21" s="255"/>
-      <c r="N21" s="255"/>
-      <c r="O21" s="255"/>
-      <c r="P21" s="256"/>
+      <c r="B21" s="234"/>
+      <c r="C21" s="234"/>
+      <c r="D21" s="234"/>
+      <c r="E21" s="234"/>
+      <c r="F21" s="234"/>
+      <c r="G21" s="234"/>
+      <c r="H21" s="234"/>
+      <c r="I21" s="234"/>
+      <c r="J21" s="234"/>
+      <c r="K21" s="234"/>
+      <c r="L21" s="234"/>
+      <c r="M21" s="234"/>
+      <c r="N21" s="234"/>
+      <c r="O21" s="234"/>
+      <c r="P21" s="235"/>
       <c r="AP21"/>
       <c r="AQ21"/>
       <c r="AR21"/>
       <c r="AS21"/>
     </row>
     <row r="22" spans="1:51" ht="24" thickBot="1">
-      <c r="A22" s="239" t="s">
+      <c r="A22" s="244" t="s">
         <v>331</v>
       </c>
-      <c r="B22" s="240"/>
-      <c r="C22" s="241"/>
-      <c r="D22" s="237" t="s">
+      <c r="B22" s="242"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="239" t="s">
         <v>334</v>
       </c>
-      <c r="E22" s="263" t="s">
+      <c r="E22" s="241" t="s">
         <v>332</v>
       </c>
-      <c r="F22" s="240"/>
-      <c r="G22" s="240"/>
-      <c r="H22" s="240"/>
-      <c r="I22" s="241"/>
-      <c r="J22" s="237" t="s">
+      <c r="F22" s="242"/>
+      <c r="G22" s="242"/>
+      <c r="H22" s="242"/>
+      <c r="I22" s="243"/>
+      <c r="J22" s="239" t="s">
         <v>334</v>
       </c>
-      <c r="K22" s="260" t="s">
+      <c r="K22" s="236" t="s">
         <v>333</v>
       </c>
-      <c r="L22" s="261"/>
-      <c r="M22" s="261"/>
-      <c r="N22" s="261"/>
-      <c r="O22" s="261"/>
-      <c r="P22" s="262"/>
+      <c r="L22" s="237"/>
+      <c r="M22" s="237"/>
+      <c r="N22" s="237"/>
+      <c r="O22" s="237"/>
+      <c r="P22" s="238"/>
       <c r="AM22"/>
       <c r="AN22"/>
       <c r="AO22"/>
@@ -43303,7 +43456,7 @@
       <c r="C23" s="79" t="s">
         <v>397</v>
       </c>
-      <c r="D23" s="237"/>
+      <c r="D23" s="239"/>
       <c r="E23" s="79" t="s">
         <v>396</v>
       </c>
@@ -43315,7 +43468,7 @@
       </c>
       <c r="H23" s="84"/>
       <c r="I23" s="85"/>
-      <c r="J23" s="237"/>
+      <c r="J23" s="239"/>
       <c r="K23" s="79" t="s">
         <v>578</v>
       </c>
@@ -43348,7 +43501,7 @@
       <c r="C24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="237"/>
+      <c r="D24" s="239"/>
       <c r="E24" s="34" t="s">
         <v>16</v>
       </c>
@@ -43364,7 +43517,7 @@
       <c r="I24" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J24" s="237"/>
+      <c r="J24" s="239"/>
       <c r="K24" s="34" t="s">
         <v>18</v>
       </c>
@@ -43400,7 +43553,7 @@
       <c r="C25" s="17">
         <v>45</v>
       </c>
-      <c r="D25" s="237"/>
+      <c r="D25" s="239"/>
       <c r="E25" s="17">
         <v>35</v>
       </c>
@@ -43416,7 +43569,7 @@
       <c r="I25" s="17">
         <v>95</v>
       </c>
-      <c r="J25" s="237"/>
+      <c r="J25" s="239"/>
       <c r="K25" s="17">
         <v>2.5</v>
       </c>
@@ -43443,30 +43596,30 @@
       <c r="AS25"/>
     </row>
     <row r="26" spans="1:51" ht="50.25" customHeight="1" thickBot="1">
-      <c r="A26" s="248" t="s">
+      <c r="A26" s="258" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="242"/>
-      <c r="C26" s="242"/>
-      <c r="D26" s="238"/>
-      <c r="E26" s="242" t="s">
+      <c r="B26" s="252"/>
+      <c r="C26" s="252"/>
+      <c r="D26" s="240"/>
+      <c r="E26" s="252" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="242"/>
-      <c r="G26" s="242"/>
+      <c r="F26" s="252"/>
+      <c r="G26" s="252"/>
       <c r="H26" s="45" t="s">
         <v>36</v>
       </c>
       <c r="I26" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="J26" s="238"/>
-      <c r="K26" s="249" t="s">
+      <c r="J26" s="240"/>
+      <c r="K26" s="259" t="s">
         <v>38</v>
       </c>
-      <c r="L26" s="249"/>
-      <c r="M26" s="249"/>
-      <c r="N26" s="249"/>
+      <c r="L26" s="259"/>
+      <c r="M26" s="259"/>
+      <c r="N26" s="259"/>
       <c r="O26" s="45" t="s">
         <v>36</v>
       </c>
@@ -43487,53 +43640,53 @@
     </row>
     <row r="29" spans="1:51" ht="15" thickBot="1"/>
     <row r="30" spans="1:51" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A30" s="230" t="s">
+      <c r="A30" s="245" t="s">
         <v>576</v>
       </c>
-      <c r="B30" s="231"/>
-      <c r="C30" s="231"/>
-      <c r="D30" s="231"/>
-      <c r="E30" s="231"/>
-      <c r="F30" s="231"/>
-      <c r="G30" s="231"/>
-      <c r="H30" s="231"/>
-      <c r="I30" s="231"/>
-      <c r="J30" s="231"/>
-      <c r="K30" s="231"/>
-      <c r="L30" s="231"/>
-      <c r="M30" s="231"/>
-      <c r="N30" s="231"/>
-      <c r="O30" s="231"/>
-      <c r="P30" s="231"/>
-      <c r="Q30" s="231"/>
-      <c r="R30" s="231"/>
-      <c r="S30" s="231"/>
-      <c r="T30" s="231"/>
-      <c r="U30" s="231"/>
-      <c r="V30" s="231"/>
-      <c r="W30" s="231"/>
-      <c r="X30" s="231"/>
-      <c r="Y30" s="231"/>
-      <c r="Z30" s="231"/>
-      <c r="AA30" s="231"/>
-      <c r="AB30" s="231"/>
-      <c r="AC30" s="231"/>
-      <c r="AD30" s="231"/>
-      <c r="AE30" s="231"/>
-      <c r="AF30" s="231"/>
-      <c r="AG30" s="231"/>
-      <c r="AH30" s="231"/>
-      <c r="AI30" s="231"/>
-      <c r="AJ30" s="231"/>
-      <c r="AK30" s="231"/>
-      <c r="AL30" s="231"/>
-      <c r="AM30" s="231"/>
-      <c r="AN30" s="231"/>
-      <c r="AO30" s="231"/>
-      <c r="AP30" s="231"/>
-      <c r="AQ30" s="231"/>
-      <c r="AR30" s="231"/>
-      <c r="AS30" s="232"/>
+      <c r="B30" s="246"/>
+      <c r="C30" s="246"/>
+      <c r="D30" s="246"/>
+      <c r="E30" s="246"/>
+      <c r="F30" s="246"/>
+      <c r="G30" s="246"/>
+      <c r="H30" s="246"/>
+      <c r="I30" s="246"/>
+      <c r="J30" s="246"/>
+      <c r="K30" s="246"/>
+      <c r="L30" s="246"/>
+      <c r="M30" s="246"/>
+      <c r="N30" s="246"/>
+      <c r="O30" s="246"/>
+      <c r="P30" s="246"/>
+      <c r="Q30" s="246"/>
+      <c r="R30" s="246"/>
+      <c r="S30" s="246"/>
+      <c r="T30" s="246"/>
+      <c r="U30" s="246"/>
+      <c r="V30" s="246"/>
+      <c r="W30" s="246"/>
+      <c r="X30" s="246"/>
+      <c r="Y30" s="246"/>
+      <c r="Z30" s="246"/>
+      <c r="AA30" s="246"/>
+      <c r="AB30" s="246"/>
+      <c r="AC30" s="246"/>
+      <c r="AD30" s="246"/>
+      <c r="AE30" s="246"/>
+      <c r="AF30" s="246"/>
+      <c r="AG30" s="246"/>
+      <c r="AH30" s="246"/>
+      <c r="AI30" s="246"/>
+      <c r="AJ30" s="246"/>
+      <c r="AK30" s="246"/>
+      <c r="AL30" s="246"/>
+      <c r="AM30" s="246"/>
+      <c r="AN30" s="246"/>
+      <c r="AO30" s="246"/>
+      <c r="AP30" s="246"/>
+      <c r="AQ30" s="246"/>
+      <c r="AR30" s="246"/>
+      <c r="AS30" s="247"/>
     </row>
     <row r="31" spans="1:51" s="23" customFormat="1" ht="30.75" customHeight="1">
       <c r="A31" s="78" t="s">
@@ -44187,14 +44340,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="K22:P22"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="A30:AS30"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="K8:T8"/>
@@ -44211,6 +44356,14 @@
     <mergeCell ref="K18:N18"/>
     <mergeCell ref="A19:P20"/>
     <mergeCell ref="A21:P21"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="K22:P22"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>